<commit_message>
cambio de liberias para exportar solicitudes a excel y exportacion de solicitudes autorizadas
</commit_message>
<xml_diff>
--- a/public/Solicitudes.xlsx
+++ b/public/Solicitudes.xlsx
@@ -15,105 +15,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12">
   <si>
     <t>#</t>
   </si>
   <si>
-    <t>ID Usuario</t>
-  </si>
-  <si>
-    <t>Tipo Solicitud</t>
-  </si>
-  <si>
-    <t>Pago</t>
-  </si>
-  <si>
-    <t>Fecha Ausencia</t>
-  </si>
-  <si>
-    <t>Fecha Reingreso</t>
-  </si>
-  <si>
-    <t>Motivo</t>
-  </si>
-  <si>
-    <t>ID Jefe</t>
-  </si>
-  <si>
-    <t>Jefe Status</t>
-  </si>
-  <si>
-    <t>RH Status</t>
-  </si>
-  <si>
-    <t>Creado</t>
-  </si>
-  <si>
-    <t>Ultima modificacion</t>
-  </si>
-  <si>
-    <t>Salir durante la Jornada</t>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>Apellidos</t>
+  </si>
+  <si>
+    <t>Tipo solicitud</t>
+  </si>
+  <si>
+    <t>Forma de pago</t>
+  </si>
+  <si>
+    <t>Fechas de ausencia</t>
+  </si>
+  <si>
+    <t>Vacaciones restantes</t>
+  </si>
+  <si>
+    <t>Solicitar vacaciones</t>
+  </si>
+  <si>
+    <t>A cuenta de vacaciones</t>
+  </si>
+  <si>
+    <t>Salir durante la jornada</t>
   </si>
   <si>
     <t>Pagar Tiempo/Dia</t>
   </si>
   <si>
-    <t>2021-12-23</t>
-  </si>
-  <si>
-    <t>2021-12-31</t>
-  </si>
-  <si>
-    <t>fchjnb jknk,</t>
-  </si>
-  <si>
-    <t>Pendiente</t>
-  </si>
-  <si>
-    <t>2021-12-16T19:04:05.000000Z</t>
-  </si>
-  <si>
-    <t>2021-12-16</t>
-  </si>
-  <si>
-    <t>2021-12-22</t>
-  </si>
-  <si>
-    <t>dgdfcgb</t>
-  </si>
-  <si>
-    <t>2021-12-16T19:18:11.000000Z</t>
-  </si>
-  <si>
     <t>Faltar a sus labores</t>
-  </si>
-  <si>
-    <t>2021-12-17</t>
-  </si>
-  <si>
-    <t>2021-12-30</t>
-  </si>
-  <si>
-    <t>vecccccdfgrt</t>
-  </si>
-  <si>
-    <t>2021-12-16T19:18:26.000000Z</t>
-  </si>
-  <si>
-    <t>A cuenta de vacaciones</t>
-  </si>
-  <si>
-    <t>2021-12-08</t>
-  </si>
-  <si>
-    <t>2021-12-24</t>
-  </si>
-  <si>
-    <t>zxtgyggu</t>
-  </si>
-  <si>
-    <t>2021-12-16T19:18:47.000000Z</t>
   </si>
 </sst>
 </file>
@@ -452,7 +389,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,20 +398,15 @@
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="2.285156" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="12.854004" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="29.421387" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="26.993408" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="17.567139" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="18.709717" bestFit="true" customWidth="true" style="0"/>
-    <col min="7" max="7" width="15.281982" bestFit="true" customWidth="true" style="0"/>
-    <col min="8" max="8" width="9.283447" bestFit="true" customWidth="true" style="0"/>
-    <col min="9" max="9" width="13.996582" bestFit="true" customWidth="true" style="0"/>
-    <col min="10" max="10" width="11.711426" bestFit="true" customWidth="true" style="0"/>
-    <col min="11" max="11" width="32.991943" bestFit="true" customWidth="true" style="0"/>
-    <col min="12" max="12" width="32.991943" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="8.140869" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="11.711426" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="29.421387" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="26.993408" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="22.280273" bestFit="true" customWidth="true" style="0"/>
+    <col min="7" max="7" width="24.708252" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -496,172 +428,38 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L2" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J3" t="s">
-        <v>17</v>
-      </c>
-      <c r="K3" t="s">
-        <v>22</v>
-      </c>
-      <c r="L3" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>23</v>
-      </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4" t="s">
-        <v>17</v>
-      </c>
-      <c r="J4" t="s">
-        <v>17</v>
-      </c>
-      <c r="K4" t="s">
-        <v>27</v>
-      </c>
-      <c r="L4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F5" t="s">
-        <v>30</v>
-      </c>
-      <c r="G5" t="s">
-        <v>31</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-      <c r="I5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J5" t="s">
-        <v>17</v>
-      </c>
-      <c r="K5" t="s">
-        <v>32</v>
-      </c>
-      <c r="L5" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>